<commit_message>
Change owner to row_owner
</commit_message>
<xml_diff>
--- a/app/config/tables/farms/forms/farms/farms.xlsx
+++ b/app/config/tables/farms/forms/farms/farms.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\farms\forms\farms\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4687" yWindow="6401" windowWidth="25606" windowHeight="16063" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4680" yWindow="6400" windowWidth="35880" windowHeight="17500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -288,14 +283,14 @@
   </si>
   <si>
     <t>_.map(context, function(place){
-return { data_value = place.city, state: place.state, display: {title: {text: place.city} } };
+return { data_value:place.city, state: place.state, display: {title: {text: place.city} } };
 })</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -977,16 +972,16 @@
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="49.5" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +1010,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1027,7 +1022,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1037,7 +1032,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>55</v>
       </c>
@@ -1049,7 +1044,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1059,7 +1054,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1069,7 +1064,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="5"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1079,7 +1074,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1090,7 +1085,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
@@ -1099,7 +1094,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1110,7 +1105,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1121,7 +1116,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1132,7 +1127,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1143,7 +1138,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1154,69 +1149,69 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="C19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="C20" s="2"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32" s="6"/>
       <c r="B32" s="3"/>
     </row>
@@ -1239,14 +1234,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="19" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1252,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1266,7 +1261,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1270,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1284,7 +1279,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1293,7 +1288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1301,7 +1296,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -1309,7 +1304,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1333,17 +1328,17 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
-    <col min="7" max="8" width="42.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="8" width="42.83203125" customWidth="1"/>
     <col min="10" max="10" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
@@ -1375,7 +1370,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>58</v>
       </c>
@@ -1401,7 +1396,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="78.55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="78.5">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -1421,7 +1416,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1435,7 +1430,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
@@ -1464,9 +1459,9 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1483,7 +1478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1500,16 +1495,16 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="E14" s="6"/>
     </row>
   </sheetData>
@@ -1531,14 +1526,14 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1573,7 +1568,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="31.5">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -1592,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
@@ -1605,7 +1600,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="31.5">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -1622,7 +1617,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="31.5">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
@@ -1639,7 +1634,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="31.5">
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1673,13 +1668,13 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="8" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="30.109375" customWidth="1"/>
+    <col min="6" max="8" width="17.83203125" customWidth="1"/>
+    <col min="10" max="10" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1711,7 +1706,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="62.75">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -1729,7 +1724,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="31.5">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
@@ -1768,12 +1763,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="61.109375" customWidth="1"/>
+    <col min="2" max="2" width="61.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -1781,7 +1776,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="81" customHeight="1">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1789,40 +1784,40 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="17">
       <c r="B5" s="13"/>
     </row>
-    <row r="6" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="17">
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="17">
       <c r="B7" s="14"/>
     </row>
-    <row r="8" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="17">
       <c r="B8" s="14"/>
     </row>
-    <row r="9" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="17">
       <c r="B9" s="14"/>
     </row>
-    <row r="10" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="17">
       <c r="B10" s="14"/>
     </row>
-    <row r="11" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="17">
       <c r="B11" s="14"/>
     </row>
-    <row r="12" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="17">
       <c r="B12" s="14"/>
     </row>
-    <row r="13" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="17">
       <c r="B13" s="14"/>
     </row>
-    <row r="14" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="17">
       <c r="B14" s="14"/>
     </row>
-    <row r="15" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="17">
       <c r="B15" s="14"/>
     </row>
-    <row r="16" spans="1:2" ht="17.05" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="17">
       <c r="B16" s="14"/>
     </row>
   </sheetData>
@@ -1844,9 +1839,9 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
@@ -1854,7 +1849,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -1862,7 +1857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
@@ -1870,7 +1865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
         <v>47</v>
       </c>
@@ -1878,7 +1873,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
         <v>48</v>
       </c>
@@ -1886,7 +1881,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="31.5">
       <c r="A6" s="6" t="s">
         <v>72</v>
       </c>
@@ -1894,7 +1889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="31.5">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1902,7 +1897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="31.5">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>

</xml_diff>